<commit_message>
fix codebook for refused
</commit_message>
<xml_diff>
--- a/metadata/SDD-NHANES-BPQ.xlsx
+++ b/metadata/SDD-NHANES-BPQ.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3538D0AE-3D99-5D4C-ADBC-2D42A60E1A83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59891858-7A3D-4C49-8B20-0A7E5205C0A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-580" yWindow="-15780" windowWidth="25640" windowHeight="13760" activeTab="5" xr2:uid="{58E4DFD5-BA0B-AC44-8A63-99A3E8BCBB5B}"/>
   </bookViews>
@@ -837,7 +837,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,7 +896,7 @@
         <v>61</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>54</v>

</xml_diff>